<commit_message>
Memperbaiki struktur penduduk dan beberapa master data
</commit_message>
<xml_diff>
--- a/public/assets/dashboard/file/format_import_penduduk.xlsx
+++ b/public/assets/dashboard/file/format_import_penduduk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hiday\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C077109-4363-4124-A988-43C55AA8241A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FDBAD1-150B-4AE3-A90C-F3B6E2F00DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{8DC2C78B-9B07-4471-88C4-9E6C8ED1AA7D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Nama</t>
   </si>
@@ -44,40 +44,13 @@
     <t>Jenis Kelamin</t>
   </si>
   <si>
-    <t>Tempat Lahir</t>
-  </si>
-  <si>
     <t>Tanggal Lahir</t>
   </si>
   <si>
-    <t>Agama</t>
-  </si>
-  <si>
     <t>Status Pendidikan Terakhir</t>
   </si>
   <si>
     <t>Pekerjaan</t>
-  </si>
-  <si>
-    <t>Golongan Darah</t>
-  </si>
-  <si>
-    <t>Status Perkawinan</t>
-  </si>
-  <si>
-    <t>Tanggal Perkawinan</t>
-  </si>
-  <si>
-    <t>Kewarganegaraan</t>
-  </si>
-  <si>
-    <t>Nomor Paspor</t>
-  </si>
-  <si>
-    <t>Nomor Kitap</t>
-  </si>
-  <si>
-    <t>Alamat</t>
   </si>
   <si>
     <t>Desa</t>
@@ -456,15 +429,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{530E1333-059C-4892-990A-1777658CE914}">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:P1"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" customWidth="1"/>
+    <col min="5" max="5" width="27" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -485,33 +465,6 @@
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>